<commit_message>
Read in all cards.
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0151CCE-B77D-4D3C-8401-632EF296BA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBE88D3-5EA5-4112-A616-568245127FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>T3</t>
-  </si>
-  <si>
-    <t>2A</t>
   </si>
   <si>
     <t>Burrower</t>
@@ -1206,7 +1203,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L49"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1219,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1252,7 +1249,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1279,7 +1276,7 @@
       </c>
       <c r="L2">
         <f ca="1">RANDBETWEEN(1000,999999)</f>
-        <v>164054</v>
+        <v>7274</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1302,11 +1299,11 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L49" ca="1" si="0">RANDBETWEEN(1000,999999)</f>
-        <v>72286</v>
+        <v>964584</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1314,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1326,17 +1323,17 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>525232</v>
+        <v>658608</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1356,14 +1353,14 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>928975</v>
+        <v>357860</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1371,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1383,17 +1380,17 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>587617</v>
+        <v>671153</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1401,10 +1398,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1416,17 +1413,17 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>806719</v>
+        <v>397939</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1434,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1449,14 +1446,14 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>198249</v>
+        <v>891944</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1464,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1479,14 +1476,14 @@
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>769116</v>
+        <v>710986</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1494,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1506,14 +1503,14 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>837643</v>
+        <v>247887</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1521,10 +1518,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1536,14 +1533,14 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>521576</v>
+        <v>552084</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1551,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1563,17 +1560,17 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>832679</v>
+        <v>218476</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1581,10 +1578,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1599,17 +1596,17 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>84841</v>
+        <v>602854</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1617,29 +1614,29 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="0"/>
-        <v>619219</v>
+        <v>222540</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1647,13 +1644,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1662,14 +1659,14 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
-        <v>516483</v>
+        <v>589614</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1677,13 +1674,13 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1692,14 +1689,14 @@
         <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
-        <v>985344</v>
+        <v>561438</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1707,26 +1704,26 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="0"/>
-        <v>931487</v>
+        <v>966502</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1734,29 +1731,29 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
       <c r="J18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="0"/>
-        <v>905272</v>
+        <v>946279</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1764,13 +1761,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1779,11 +1776,11 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="0"/>
-        <v>519730</v>
+        <v>286961</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1791,26 +1788,26 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="0"/>
-        <v>233436</v>
+        <v>308153</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1818,13 +1815,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -1833,14 +1830,14 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="0"/>
-        <v>134139</v>
+        <v>98235</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1848,29 +1845,29 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="0"/>
-        <v>958360</v>
+        <v>297542</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1878,13 +1875,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -1893,17 +1890,17 @@
         <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="0"/>
-        <v>998000</v>
+        <v>40670</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1911,13 +1908,13 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -1926,14 +1923,14 @@
         <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="0"/>
-        <v>473354</v>
+        <v>274897</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1941,13 +1938,13 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1956,11 +1953,11 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="0"/>
-        <v>425008</v>
+        <v>349773</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1968,29 +1965,29 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="0"/>
-        <v>240581</v>
+        <v>678544</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1998,26 +1995,26 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E27">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="0"/>
-        <v>518961</v>
+        <v>253892</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2025,26 +2022,26 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="0"/>
-        <v>796339</v>
+        <v>491429</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2052,29 +2049,29 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29">
         <v>5</v>
       </c>
       <c r="H29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" t="s">
         <v>61</v>
       </c>
-      <c r="I29" t="s">
-        <v>62</v>
-      </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="0"/>
-        <v>49925</v>
+        <v>278821</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2082,29 +2079,29 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30">
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="0"/>
-        <v>822649</v>
+        <v>762911</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2112,13 +2109,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -2127,14 +2124,14 @@
         <v>6</v>
       </c>
       <c r="H31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="0"/>
-        <v>931431</v>
+        <v>743894</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2142,29 +2139,29 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="0"/>
-        <v>815284</v>
+        <v>327888</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2172,13 +2169,13 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -2187,14 +2184,14 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="0"/>
-        <v>581349</v>
+        <v>905838</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2202,13 +2199,13 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34">
         <v>7</v>
@@ -2217,17 +2214,17 @@
         <v>5</v>
       </c>
       <c r="H34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="0"/>
-        <v>675674</v>
+        <v>931894</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2235,26 +2232,26 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35">
         <v>6</v>
       </c>
       <c r="H35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="0"/>
-        <v>834361</v>
+        <v>984863</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2262,29 +2259,29 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>73</v>
       </c>
       <c r="E36">
         <v>7</v>
       </c>
       <c r="H36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" t="s">
         <v>74</v>
       </c>
-      <c r="I36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" t="s">
-        <v>75</v>
-      </c>
       <c r="L36">
         <f t="shared" ca="1" si="0"/>
-        <v>699616</v>
+        <v>850011</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2292,26 +2289,26 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37">
         <v>5</v>
       </c>
       <c r="H37" t="s">
+        <v>76</v>
+      </c>
+      <c r="J37" t="s">
         <v>77</v>
       </c>
-      <c r="J37" t="s">
-        <v>78</v>
-      </c>
       <c r="L37">
         <f t="shared" ca="1" si="0"/>
-        <v>135311</v>
+        <v>871916</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2319,26 +2316,26 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L38">
         <f t="shared" ca="1" si="0"/>
-        <v>969998</v>
+        <v>549459</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2346,26 +2343,26 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39">
         <v>6</v>
       </c>
       <c r="H39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L39">
         <f t="shared" ca="1" si="0"/>
-        <v>370668</v>
+        <v>342555</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2373,13 +2370,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -2388,17 +2385,17 @@
         <v>5</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L40">
         <f t="shared" ca="1" si="0"/>
-        <v>266613</v>
+        <v>992716</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2406,13 +2403,13 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2421,14 +2418,14 @@
         <v>15</v>
       </c>
       <c r="I41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L41">
         <f t="shared" ca="1" si="0"/>
-        <v>236571</v>
+        <v>654157</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2436,13 +2433,13 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -2451,14 +2448,14 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L42">
         <f t="shared" ca="1" si="0"/>
-        <v>260485</v>
+        <v>171059</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,13 +2463,13 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -2481,11 +2478,11 @@
         <v>15</v>
       </c>
       <c r="I43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L43">
         <f t="shared" ca="1" si="0"/>
-        <v>342696</v>
+        <v>632543</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2493,13 +2490,13 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -2508,17 +2505,17 @@
         <v>4</v>
       </c>
       <c r="H44" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" t="s">
         <v>90</v>
       </c>
-      <c r="I44" t="s">
-        <v>91</v>
-      </c>
       <c r="K44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L44">
         <f t="shared" ca="1" si="0"/>
-        <v>345367</v>
+        <v>584255</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2526,26 +2523,26 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E45">
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L45">
         <f t="shared" ca="1" si="0"/>
-        <v>589465</v>
+        <v>428391</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2553,13 +2550,13 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E46">
         <v>8</v>
@@ -2571,11 +2568,11 @@
         <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L46">
         <f t="shared" ca="1" si="0"/>
-        <v>747768</v>
+        <v>195753</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2583,68 +2580,68 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
         <v>96</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="s">
-        <v>97</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L47">
         <f t="shared" ca="1" si="0"/>
-        <v>982232</v>
+        <v>123502</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L48">
         <f t="shared" ca="1" si="0"/>
-        <v>61414</v>
+        <v>460362</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" t="s">
         <v>99</v>
       </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="s">
-        <v>97</v>
-      </c>
-      <c r="H49" t="s">
-        <v>100</v>
-      </c>
       <c r="L49">
         <f t="shared" ca="1" si="0"/>
-        <v>690389</v>
+        <v>705634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP - setup bosses from file.
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBE88D3-5EA5-4112-A616-568245127FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B8742F-717C-4F68-9A54-8D39C1746826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -337,13 +337,157 @@
   </si>
   <si>
     <t>ScrapBonuses</t>
+  </si>
+  <si>
+    <t>Borg1</t>
+  </si>
+  <si>
+    <t>Borg3</t>
+  </si>
+  <si>
+    <t>Borg2</t>
+  </si>
+  <si>
+    <t>Mech3</t>
+  </si>
+  <si>
+    <t>Mech1</t>
+  </si>
+  <si>
+    <t>Mech2</t>
+  </si>
+  <si>
+    <t>Necro2</t>
+  </si>
+  <si>
+    <t>Necro3</t>
+  </si>
+  <si>
+    <t>Necro1</t>
+  </si>
+  <si>
+    <t>Mage1</t>
+  </si>
+  <si>
+    <t>Mage3</t>
+  </si>
+  <si>
+    <t>Borg4</t>
+  </si>
+  <si>
+    <t>Borg5</t>
+  </si>
+  <si>
+    <t>Borg6</t>
+  </si>
+  <si>
+    <t>Borg7</t>
+  </si>
+  <si>
+    <t>Borg8</t>
+  </si>
+  <si>
+    <t>Borg9</t>
+  </si>
+  <si>
+    <t>Borg10</t>
+  </si>
+  <si>
+    <t>Borg11</t>
+  </si>
+  <si>
+    <t>Borg12</t>
+  </si>
+  <si>
+    <t>Mech4</t>
+  </si>
+  <si>
+    <t>Mech5</t>
+  </si>
+  <si>
+    <t>Mech6</t>
+  </si>
+  <si>
+    <t>Mech7</t>
+  </si>
+  <si>
+    <t>Mech8</t>
+  </si>
+  <si>
+    <t>Mech9</t>
+  </si>
+  <si>
+    <t>Mech10</t>
+  </si>
+  <si>
+    <t>Mech11</t>
+  </si>
+  <si>
+    <t>Mage5</t>
+  </si>
+  <si>
+    <t>Mage6</t>
+  </si>
+  <si>
+    <t>Necro4</t>
+  </si>
+  <si>
+    <t>Necro5</t>
+  </si>
+  <si>
+    <t>Necro6</t>
+  </si>
+  <si>
+    <t>Necro7</t>
+  </si>
+  <si>
+    <t>Necro8</t>
+  </si>
+  <si>
+    <t>Necro9</t>
+  </si>
+  <si>
+    <t>Necro10</t>
+  </si>
+  <si>
+    <t>Necro11</t>
+  </si>
+  <si>
+    <t>Mage4</t>
+  </si>
+  <si>
+    <t>Mage2</t>
+  </si>
+  <si>
+    <t>Mage7</t>
+  </si>
+  <si>
+    <t>Mage8</t>
+  </si>
+  <si>
+    <t>Mage9</t>
+  </si>
+  <si>
+    <t>Mage10</t>
+  </si>
+  <si>
+    <t>Mage11</t>
+  </si>
+  <si>
+    <t>Neutral2</t>
+  </si>
+  <si>
+    <t>Neutral1</t>
+  </si>
+  <si>
+    <t>Neutral3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +618,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -867,7 +1017,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -895,9 +1049,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="GuildBonuses"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="AllyBonuses"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ScrapBonuses"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Id">
-      <calculatedColumnFormula>RANDBETWEEN(1000,999999)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Id" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1202,13 +1354,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
@@ -1274,9 +1427,8 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="L2">
-        <f ca="1">RANDBETWEEN(1000,999999)</f>
-        <v>7274</v>
+      <c r="L2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1301,9 +1453,8 @@
       <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L49" ca="1" si="0">RANDBETWEEN(1000,999999)</f>
-        <v>964584</v>
+      <c r="L3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1331,9 +1482,8 @@
       <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="L4">
-        <f t="shared" ca="1" si="0"/>
-        <v>658608</v>
+      <c r="L4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1358,9 +1508,8 @@
       <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="L5">
-        <f t="shared" ca="1" si="0"/>
-        <v>357860</v>
+      <c r="L5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1388,9 +1537,8 @@
       <c r="J6" t="s">
         <v>24</v>
       </c>
-      <c r="L6">
-        <f t="shared" ca="1" si="0"/>
-        <v>671153</v>
+      <c r="L6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1421,9 +1569,8 @@
       <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="L7">
-        <f t="shared" ca="1" si="0"/>
-        <v>397939</v>
+      <c r="L7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1451,9 +1598,8 @@
       <c r="J8" t="s">
         <v>24</v>
       </c>
-      <c r="L8">
-        <f t="shared" ca="1" si="0"/>
-        <v>891944</v>
+      <c r="L8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1481,9 +1627,8 @@
       <c r="I9" t="s">
         <v>27</v>
       </c>
-      <c r="L9">
-        <f t="shared" ca="1" si="0"/>
-        <v>710986</v>
+      <c r="L9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1508,9 +1653,8 @@
       <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="L10">
-        <f t="shared" ca="1" si="0"/>
-        <v>247887</v>
+      <c r="L10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1538,9 +1682,8 @@
       <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="L11">
-        <f t="shared" ca="1" si="0"/>
-        <v>552084</v>
+      <c r="L11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1568,9 +1711,8 @@
       <c r="K12" t="s">
         <v>34</v>
       </c>
-      <c r="L12">
-        <f t="shared" ca="1" si="0"/>
-        <v>218476</v>
+      <c r="L12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1604,9 +1746,8 @@
       <c r="J13" t="s">
         <v>24</v>
       </c>
-      <c r="L13">
-        <f t="shared" ca="1" si="0"/>
-        <v>602854</v>
+      <c r="L13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1634,9 +1775,8 @@
       <c r="K14" t="s">
         <v>33</v>
       </c>
-      <c r="L14">
-        <f t="shared" ca="1" si="0"/>
-        <v>222540</v>
+      <c r="L14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1664,9 +1804,8 @@
       <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="L15">
-        <f t="shared" ca="1" si="0"/>
-        <v>589614</v>
+      <c r="L15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1694,9 +1833,8 @@
       <c r="I16" t="s">
         <v>33</v>
       </c>
-      <c r="L16">
-        <f t="shared" ca="1" si="0"/>
-        <v>561438</v>
+      <c r="L16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1721,9 +1859,8 @@
       <c r="I17" t="s">
         <v>40</v>
       </c>
-      <c r="L17">
-        <f t="shared" ca="1" si="0"/>
-        <v>966502</v>
+      <c r="L17" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,9 +1888,8 @@
       <c r="J18" t="s">
         <v>44</v>
       </c>
-      <c r="L18">
-        <f t="shared" ca="1" si="0"/>
-        <v>946279</v>
+      <c r="L18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1778,9 +1914,8 @@
       <c r="H19" t="s">
         <v>34</v>
       </c>
-      <c r="L19">
-        <f t="shared" ca="1" si="0"/>
-        <v>286961</v>
+      <c r="L19" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1805,9 +1940,8 @@
       <c r="I20" t="s">
         <v>44</v>
       </c>
-      <c r="L20">
-        <f t="shared" ca="1" si="0"/>
-        <v>308153</v>
+      <c r="L20" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1835,9 +1969,8 @@
       <c r="I21" t="s">
         <v>18</v>
       </c>
-      <c r="L21">
-        <f t="shared" ca="1" si="0"/>
-        <v>98235</v>
+      <c r="L21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1865,9 +1998,8 @@
       <c r="J22" t="s">
         <v>40</v>
       </c>
-      <c r="L22">
-        <f t="shared" ca="1" si="0"/>
-        <v>297542</v>
+      <c r="L22" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1898,9 +2030,8 @@
       <c r="J23" t="s">
         <v>31</v>
       </c>
-      <c r="L23">
-        <f t="shared" ca="1" si="0"/>
-        <v>40670</v>
+      <c r="L23" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1928,9 +2059,8 @@
       <c r="K24" t="s">
         <v>40</v>
       </c>
-      <c r="L24">
-        <f t="shared" ca="1" si="0"/>
-        <v>274897</v>
+      <c r="L24" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1955,9 +2085,8 @@
       <c r="H25" t="s">
         <v>18</v>
       </c>
-      <c r="L25">
-        <f t="shared" ca="1" si="0"/>
-        <v>349773</v>
+      <c r="L25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1985,9 +2114,8 @@
       <c r="J26" t="s">
         <v>55</v>
       </c>
-      <c r="L26">
-        <f t="shared" ca="1" si="0"/>
-        <v>678544</v>
+      <c r="L26" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2012,9 +2140,8 @@
       <c r="J27" t="s">
         <v>27</v>
       </c>
-      <c r="L27">
-        <f t="shared" ca="1" si="0"/>
-        <v>253892</v>
+      <c r="L27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2039,9 +2166,8 @@
       <c r="I28" t="s">
         <v>18</v>
       </c>
-      <c r="L28">
-        <f t="shared" ca="1" si="0"/>
-        <v>491429</v>
+      <c r="L28" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2069,9 +2195,8 @@
       <c r="J29" t="s">
         <v>18</v>
       </c>
-      <c r="L29">
-        <f t="shared" ca="1" si="0"/>
-        <v>278821</v>
+      <c r="L29" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2099,9 +2224,8 @@
       <c r="J30" t="s">
         <v>55</v>
       </c>
-      <c r="L30">
-        <f t="shared" ca="1" si="0"/>
-        <v>762911</v>
+      <c r="L30" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2129,9 +2253,8 @@
       <c r="I31" t="s">
         <v>55</v>
       </c>
-      <c r="L31">
-        <f t="shared" ca="1" si="0"/>
-        <v>743894</v>
+      <c r="L31" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2159,9 +2282,8 @@
       <c r="J32" t="s">
         <v>18</v>
       </c>
-      <c r="L32">
-        <f t="shared" ca="1" si="0"/>
-        <v>327888</v>
+      <c r="L32" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2189,9 +2311,8 @@
       <c r="K33" t="s">
         <v>15</v>
       </c>
-      <c r="L33">
-        <f t="shared" ca="1" si="0"/>
-        <v>905838</v>
+      <c r="L33" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2222,9 +2343,8 @@
       <c r="K34" t="s">
         <v>31</v>
       </c>
-      <c r="L34">
-        <f t="shared" ca="1" si="0"/>
-        <v>931894</v>
+      <c r="L34" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2249,9 +2369,8 @@
       <c r="I35" t="s">
         <v>18</v>
       </c>
-      <c r="L35">
-        <f t="shared" ca="1" si="0"/>
-        <v>984863</v>
+      <c r="L35" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2279,9 +2398,8 @@
       <c r="J36" t="s">
         <v>74</v>
       </c>
-      <c r="L36">
-        <f t="shared" ca="1" si="0"/>
-        <v>850011</v>
+      <c r="L36" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2306,9 +2424,8 @@
       <c r="J37" t="s">
         <v>77</v>
       </c>
-      <c r="L37">
-        <f t="shared" ca="1" si="0"/>
-        <v>871916</v>
+      <c r="L37" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2333,9 +2450,8 @@
       <c r="I38" t="s">
         <v>79</v>
       </c>
-      <c r="L38">
-        <f t="shared" ca="1" si="0"/>
-        <v>549459</v>
+      <c r="L38" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2360,9 +2476,8 @@
       <c r="I39" t="s">
         <v>17</v>
       </c>
-      <c r="L39">
-        <f t="shared" ca="1" si="0"/>
-        <v>342555</v>
+      <c r="L39" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2393,9 +2508,8 @@
       <c r="J40" t="s">
         <v>83</v>
       </c>
-      <c r="L40">
-        <f t="shared" ca="1" si="0"/>
-        <v>992716</v>
+      <c r="L40" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,9 +2537,8 @@
       <c r="K41" t="s">
         <v>31</v>
       </c>
-      <c r="L41">
-        <f t="shared" ca="1" si="0"/>
-        <v>654157</v>
+      <c r="L41" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2453,9 +2566,8 @@
       <c r="K42" t="s">
         <v>86</v>
       </c>
-      <c r="L42">
-        <f t="shared" ca="1" si="0"/>
-        <v>171059</v>
+      <c r="L42" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2480,9 +2592,8 @@
       <c r="I43" t="s">
         <v>18</v>
       </c>
-      <c r="L43">
-        <f t="shared" ca="1" si="0"/>
-        <v>632543</v>
+      <c r="L43" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2513,9 +2624,8 @@
       <c r="K44" t="s">
         <v>18</v>
       </c>
-      <c r="L44">
-        <f t="shared" ca="1" si="0"/>
-        <v>584255</v>
+      <c r="L44" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2540,9 +2650,8 @@
       <c r="J45" t="s">
         <v>33</v>
       </c>
-      <c r="L45">
-        <f t="shared" ca="1" si="0"/>
-        <v>428391</v>
+      <c r="L45" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2570,9 +2679,8 @@
       <c r="H46" t="s">
         <v>94</v>
       </c>
-      <c r="L46">
-        <f t="shared" ca="1" si="0"/>
-        <v>195753</v>
+      <c r="L46" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2597,9 +2705,8 @@
       <c r="K47" t="s">
         <v>33</v>
       </c>
-      <c r="L47">
-        <f t="shared" ca="1" si="0"/>
-        <v>123502</v>
+      <c r="L47" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2618,9 +2725,8 @@
       <c r="H48" t="s">
         <v>34</v>
       </c>
-      <c r="L48">
-        <f t="shared" ca="1" si="0"/>
-        <v>460362</v>
+      <c r="L48" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2639,12 +2745,12 @@
       <c r="H49" t="s">
         <v>99</v>
       </c>
-      <c r="L49">
-        <f t="shared" ca="1" si="0"/>
-        <v>705634</v>
+      <c r="L49" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented v1 flow for setup of new player
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B8742F-717C-4F68-9A54-8D39C1746826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8469074-3DB4-488A-86E0-5A5C1454FE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -318,9 +318,6 @@
     <t>A3,T4,H5</t>
   </si>
   <si>
-    <t>Explorer</t>
-  </si>
-  <si>
     <t>Neutral</t>
   </si>
   <si>
@@ -475,9 +472,6 @@
   </si>
   <si>
     <t>Neutral2</t>
-  </si>
-  <si>
-    <t>Neutral1</t>
   </si>
   <si>
     <t>Neutral3</t>
@@ -970,8 +964,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1035,8 +1030,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L49" totalsRowShown="0">
-  <autoFilter ref="A1:L49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L48" totalsRowShown="0">
+  <autoFilter ref="A1:L48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Quantity"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
@@ -1352,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1367,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1402,7 +1397,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1428,7 +1423,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1454,7 +1449,7 @@
         <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1483,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1509,7 +1504,7 @@
         <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1538,7 +1533,7 @@
         <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1570,7 +1565,7 @@
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1599,7 +1594,7 @@
         <v>24</v>
       </c>
       <c r="L8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1628,7 +1623,7 @@
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1654,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1683,7 +1678,7 @@
         <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1712,7 +1707,7 @@
         <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1747,7 +1742,7 @@
         <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1776,7 +1771,7 @@
         <v>33</v>
       </c>
       <c r="L14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1805,7 +1800,7 @@
         <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1834,7 +1829,7 @@
         <v>33</v>
       </c>
       <c r="L16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1860,7 +1855,7 @@
         <v>40</v>
       </c>
       <c r="L17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1889,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1915,7 +1910,7 @@
         <v>34</v>
       </c>
       <c r="L19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1941,7 +1936,7 @@
         <v>44</v>
       </c>
       <c r="L20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1970,7 +1965,7 @@
         <v>18</v>
       </c>
       <c r="L21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1999,7 +1994,7 @@
         <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2031,7 +2026,7 @@
         <v>31</v>
       </c>
       <c r="L23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2060,7 +2055,7 @@
         <v>40</v>
       </c>
       <c r="L24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2086,7 +2081,7 @@
         <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2115,7 +2110,7 @@
         <v>55</v>
       </c>
       <c r="L26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2141,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2167,7 +2162,7 @@
         <v>18</v>
       </c>
       <c r="L28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2196,7 +2191,7 @@
         <v>18</v>
       </c>
       <c r="L29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2225,7 +2220,7 @@
         <v>55</v>
       </c>
       <c r="L30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2254,7 +2249,7 @@
         <v>55</v>
       </c>
       <c r="L31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2283,7 +2278,7 @@
         <v>18</v>
       </c>
       <c r="L32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2312,7 +2307,7 @@
         <v>15</v>
       </c>
       <c r="L33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2344,7 +2339,7 @@
         <v>31</v>
       </c>
       <c r="L34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2370,7 +2365,7 @@
         <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2399,7 +2394,7 @@
         <v>74</v>
       </c>
       <c r="L36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2425,7 +2420,7 @@
         <v>77</v>
       </c>
       <c r="L37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,7 +2446,7 @@
         <v>79</v>
       </c>
       <c r="L38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2477,7 +2472,7 @@
         <v>17</v>
       </c>
       <c r="L39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2509,7 +2504,7 @@
         <v>83</v>
       </c>
       <c r="L40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2538,7 +2533,7 @@
         <v>31</v>
       </c>
       <c r="L41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2567,7 +2562,7 @@
         <v>86</v>
       </c>
       <c r="L42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2593,7 +2588,7 @@
         <v>18</v>
       </c>
       <c r="L43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2625,7 +2620,7 @@
         <v>18</v>
       </c>
       <c r="L44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2651,7 +2646,7 @@
         <v>33</v>
       </c>
       <c r="L45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2680,38 +2675,32 @@
         <v>94</v>
       </c>
       <c r="L46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
         <v>95</v>
       </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
       <c r="H47" t="s">
-        <v>21</v>
-      </c>
-      <c r="K47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
         <v>97</v>
@@ -2720,33 +2709,13 @@
         <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H48" t="s">
-        <v>34</v>
-      </c>
-      <c r="L48" t="s">
+        <v>98</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="s">
-        <v>96</v>
-      </c>
-      <c r="H49" t="s">
-        <v>99</v>
-      </c>
-      <c r="L49" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>